<commit_message>
adding more density information from the foreign odor set
</commit_message>
<xml_diff>
--- a/Odor Database/odorDatabase_FINAL.xlsx
+++ b/Odor Database/odorDatabase_FINAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1380" windowWidth="45460" windowHeight="27240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="45460" windowHeight="27240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="odorDatabase_sorted_amount" sheetId="3" r:id="rId1"/>
@@ -10024,24 +10024,24 @@
   <dimension ref="A1:R199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="12"/>
     <col min="2" max="2" width="20.33203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="60.1640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="27" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="15" style="12" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="13" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="12"/>
-    <col min="10" max="10" width="18.6640625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="12" customWidth="1"/>
     <col min="11" max="11" width="12" style="12" customWidth="1"/>
     <col min="12" max="12" width="15" style="12" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="8.1640625" style="12" customWidth="1"/>
     <col min="14" max="14" width="17" style="12" customWidth="1"/>
     <col min="15" max="18" width="20.33203125" style="12" customWidth="1"/>
     <col min="19" max="16384" width="10.83203125" style="12"/>
@@ -10314,6 +10314,9 @@
       <c r="I5" s="12" t="s">
         <v>355</v>
       </c>
+      <c r="J5" s="12">
+        <v>0.8</v>
+      </c>
       <c r="K5" s="12">
         <v>154.25299999999999</v>
       </c>
@@ -10331,17 +10334,17 @@
         <f t="shared" si="1"/>
         <v>64.828560870777238</v>
       </c>
-      <c r="P5" s="29" t="e">
+      <c r="P5" s="29">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>12.5</v>
       </c>
       <c r="Q5" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="30" t="e">
+        <v>5.1862848696621793</v>
+      </c>
+      <c r="R5" s="30">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>52.328560870777238</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -10433,6 +10436,9 @@
       <c r="I7" s="12" t="s">
         <v>355</v>
       </c>
+      <c r="J7" s="12">
+        <v>0.9</v>
+      </c>
       <c r="K7" s="12">
         <v>214.34899999999999</v>
       </c>
@@ -10450,17 +10456,17 @@
         <f t="shared" si="1"/>
         <v>46.652888513592323</v>
       </c>
-      <c r="P7" s="29" t="e">
+      <c r="P7" s="29">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>11.111111111111112</v>
       </c>
       <c r="Q7" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="30" t="e">
+        <v>4.1987599662233093</v>
+      </c>
+      <c r="R7" s="30">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>35.541777402481209</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -10491,6 +10497,9 @@
       <c r="I8" s="12" t="s">
         <v>355</v>
       </c>
+      <c r="J8" s="12">
+        <v>0.8</v>
+      </c>
       <c r="K8" s="12">
         <v>296.53899999999999</v>
       </c>
@@ -10508,17 +10517,17 @@
         <f t="shared" si="1"/>
         <v>33.722377157810612</v>
       </c>
-      <c r="P8" s="29" t="e">
+      <c r="P8" s="29">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>12.5</v>
       </c>
       <c r="Q8" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="30" t="e">
+        <v>2.697790172624849</v>
+      </c>
+      <c r="R8" s="30">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>21.222377157810612</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -10610,6 +10619,9 @@
       <c r="I10" s="12" t="s">
         <v>355</v>
       </c>
+      <c r="J10" s="12">
+        <v>0.8</v>
+      </c>
       <c r="K10" s="12">
         <v>156.26900000000001</v>
       </c>
@@ -10627,17 +10639,17 @@
         <f t="shared" si="1"/>
         <v>63.992218546224784</v>
       </c>
-      <c r="P10" s="29" t="e">
+      <c r="P10" s="29">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>12.5</v>
       </c>
       <c r="Q10" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R10" s="30" t="e">
+        <v>5.1193774836979822</v>
+      </c>
+      <c r="R10" s="30">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>51.492218546224784</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>